<commit_message>
updated schedule (added schedules 4 course пн, вт, ср, сб)
</commit_message>
<xml_diff>
--- a/asuschedule/document.xlsx
+++ b/asuschedule/document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\ASU_Schedule\asuschedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BD51A0-4E82-44CE-86BB-18E35EAC15A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FB99D8-7FD8-4D0B-8578-F64F0B04229B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2270" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2488" uniqueCount="238">
   <si>
     <t>Курс</t>
   </si>
@@ -730,6 +730,33 @@
   </si>
   <si>
     <t>Киздермишов А.А.</t>
+  </si>
+  <si>
+    <t>Информационные сети и телекоммуникации</t>
+  </si>
+  <si>
+    <t>Хоконов А.Х.</t>
+  </si>
+  <si>
+    <t>Коржаков В. Е.</t>
+  </si>
+  <si>
+    <t>Шопин А.В.</t>
+  </si>
+  <si>
+    <t>Физика элементарных частиц. Стандартная модель</t>
+  </si>
+  <si>
+    <t>Электродинамические процессы</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Физика элементарныхчастиц. Стандартная модель</t>
+  </si>
+  <si>
+    <t>Копоть Л.В.</t>
   </si>
 </sst>
 </file>
@@ -2532,7 +2559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C2F2DF-FE59-47D0-BDF3-50F27700A4C2}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -2594,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2765,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2872,7 +2899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -3758,7 +3785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC10DB3-35FC-4C6A-8252-97FB7BCAAC35}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -4811,10 +4838,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059CF91E-6117-45C5-82C8-C939713C8D5E}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4913,7 +4940,124 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>233</v>
+      </c>
+      <c r="G4" t="s">
+        <v>230</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>233</v>
+      </c>
+      <c r="G5" t="s">
+        <v>230</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H6">
+        <v>327</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>178</v>
+      </c>
+      <c r="G7" t="s">
+        <v>179</v>
+      </c>
+      <c r="H7">
+        <v>404</v>
+      </c>
+      <c r="I7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9312,7 +9456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -10970,10 +11114,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11072,7 +11216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -11915,7 +12059,391 @@
         <v>1</v>
       </c>
     </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G34" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34">
+        <v>406</v>
+      </c>
+      <c r="I34" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>75</v>
+      </c>
+      <c r="G35" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35">
+        <v>324</v>
+      </c>
+      <c r="I35" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36" t="s">
+        <v>77</v>
+      </c>
+      <c r="G36" t="s">
+        <v>230</v>
+      </c>
+      <c r="H36">
+        <v>316</v>
+      </c>
+      <c r="I36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" t="s">
+        <v>231</v>
+      </c>
+      <c r="H37">
+        <v>404</v>
+      </c>
+      <c r="I37" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>79</v>
+      </c>
+      <c r="G38" t="s">
+        <v>80</v>
+      </c>
+      <c r="H38">
+        <v>405</v>
+      </c>
+      <c r="I38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>109</v>
+      </c>
+      <c r="G39" t="s">
+        <v>66</v>
+      </c>
+      <c r="H39">
+        <v>329</v>
+      </c>
+      <c r="I39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>109</v>
+      </c>
+      <c r="G40" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40">
+        <v>329</v>
+      </c>
+      <c r="I40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41" t="s">
+        <v>66</v>
+      </c>
+      <c r="H41">
+        <v>407</v>
+      </c>
+      <c r="I41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G42" t="s">
+        <v>80</v>
+      </c>
+      <c r="H42">
+        <v>405</v>
+      </c>
+      <c r="I42" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>109</v>
+      </c>
+      <c r="G43" t="s">
+        <v>66</v>
+      </c>
+      <c r="H43">
+        <v>329</v>
+      </c>
+      <c r="I43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G44" t="s">
+        <v>80</v>
+      </c>
+      <c r="H44">
+        <v>405</v>
+      </c>
+      <c r="I44" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>229</v>
+      </c>
+      <c r="G45" t="s">
+        <v>80</v>
+      </c>
+      <c r="H45">
+        <v>405</v>
+      </c>
+      <c r="I45" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46" t="s">
+        <v>68</v>
+      </c>
+      <c r="G46" t="s">
+        <v>232</v>
+      </c>
+      <c r="H46">
+        <v>511</v>
+      </c>
+      <c r="I46" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -11927,10 +12455,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11991,7 +12519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -13052,7 +13580,362 @@
         <v>1</v>
       </c>
     </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>233</v>
+      </c>
+      <c r="G40" t="s">
+        <v>230</v>
+      </c>
+      <c r="H40" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>233</v>
+      </c>
+      <c r="G41" t="s">
+        <v>230</v>
+      </c>
+      <c r="H41" t="s">
+        <v>31</v>
+      </c>
+      <c r="I41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42" t="s">
+        <v>234</v>
+      </c>
+      <c r="G42" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42">
+        <v>319</v>
+      </c>
+      <c r="I42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>109</v>
+      </c>
+      <c r="G43" t="s">
+        <v>66</v>
+      </c>
+      <c r="H43">
+        <v>329</v>
+      </c>
+      <c r="I43" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>110</v>
+      </c>
+      <c r="G44" t="s">
+        <v>232</v>
+      </c>
+      <c r="H44">
+        <v>511</v>
+      </c>
+      <c r="I44" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45" t="s">
+        <v>110</v>
+      </c>
+      <c r="G45" t="s">
+        <v>232</v>
+      </c>
+      <c r="H45">
+        <v>511</v>
+      </c>
+      <c r="I45" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" t="s">
+        <v>225</v>
+      </c>
+      <c r="H46">
+        <v>404</v>
+      </c>
+      <c r="I46" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>110</v>
+      </c>
+      <c r="G47" t="s">
+        <v>232</v>
+      </c>
+      <c r="H47">
+        <v>511</v>
+      </c>
+      <c r="I47" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>105</v>
+      </c>
+      <c r="G48" t="s">
+        <v>225</v>
+      </c>
+      <c r="H48">
+        <v>407</v>
+      </c>
+      <c r="I48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" t="s">
+        <v>85</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>110</v>
+      </c>
+      <c r="G49" t="s">
+        <v>232</v>
+      </c>
+      <c r="H49">
+        <v>511</v>
+      </c>
+      <c r="I49" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>70</v>
+      </c>
+      <c r="D50" t="s">
+        <v>85</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50" t="s">
+        <v>174</v>
+      </c>
+      <c r="G50" t="s">
+        <v>99</v>
+      </c>
+      <c r="H50">
+        <v>318</v>
+      </c>
+      <c r="I50" t="s">
+        <v>17</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+      <c r="F51" t="s">
+        <v>112</v>
+      </c>
+      <c r="G51" t="s">
+        <v>101</v>
+      </c>
+      <c r="H51">
+        <v>404</v>
+      </c>
+      <c r="I51" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -13064,10 +13947,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A50098D-1ABF-4068-8B74-18169C8AD7A1}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13166,7 +14049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -14217,7 +15100,390 @@
       <c r="F40" t="s">
         <v>86</v>
       </c>
+      <c r="I40" t="s">
+        <v>235</v>
+      </c>
       <c r="J40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G41" t="s">
+        <v>230</v>
+      </c>
+      <c r="H41" t="s">
+        <v>31</v>
+      </c>
+      <c r="I41" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>236</v>
+      </c>
+      <c r="G42" t="s">
+        <v>230</v>
+      </c>
+      <c r="H42" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>114</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>77</v>
+      </c>
+      <c r="G43" t="s">
+        <v>230</v>
+      </c>
+      <c r="H43">
+        <v>319</v>
+      </c>
+      <c r="I43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>114</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>147</v>
+      </c>
+      <c r="G44" t="s">
+        <v>80</v>
+      </c>
+      <c r="H44">
+        <v>405</v>
+      </c>
+      <c r="I44" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>147</v>
+      </c>
+      <c r="G45" t="s">
+        <v>80</v>
+      </c>
+      <c r="H45">
+        <v>328</v>
+      </c>
+      <c r="I45" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" t="s">
+        <v>114</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" t="s">
+        <v>69</v>
+      </c>
+      <c r="H46" t="s">
+        <v>96</v>
+      </c>
+      <c r="I46" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" t="s">
+        <v>114</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="F47" t="s">
+        <v>147</v>
+      </c>
+      <c r="G47" t="s">
+        <v>80</v>
+      </c>
+      <c r="H47">
+        <v>405</v>
+      </c>
+      <c r="I47" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" t="s">
+        <v>114</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>79</v>
+      </c>
+      <c r="G48" t="s">
+        <v>69</v>
+      </c>
+      <c r="H48">
+        <v>328</v>
+      </c>
+      <c r="I48" t="s">
+        <v>17</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" t="s">
+        <v>114</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>147</v>
+      </c>
+      <c r="G49" t="s">
+        <v>80</v>
+      </c>
+      <c r="H49">
+        <v>328</v>
+      </c>
+      <c r="I49" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" t="s">
+        <v>114</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>172</v>
+      </c>
+      <c r="G50" t="s">
+        <v>237</v>
+      </c>
+      <c r="H50">
+        <v>407</v>
+      </c>
+      <c r="I50" t="s">
+        <v>17</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>83</v>
+      </c>
+      <c r="D51" t="s">
+        <v>114</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>147</v>
+      </c>
+      <c r="G51" t="s">
+        <v>80</v>
+      </c>
+      <c r="H51">
+        <v>328</v>
+      </c>
+      <c r="I51" t="s">
+        <v>14</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" t="s">
+        <v>114</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>174</v>
+      </c>
+      <c r="G52" t="s">
+        <v>99</v>
+      </c>
+      <c r="H52">
+        <v>318</v>
+      </c>
+      <c r="I52" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>4</v>
+      </c>
+      <c r="B53" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" t="s">
+        <v>114</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>68</v>
+      </c>
+      <c r="G53" t="s">
+        <v>232</v>
+      </c>
+      <c r="H53">
+        <v>511</v>
+      </c>
+      <c r="I53" t="s">
+        <v>17</v>
+      </c>
+      <c r="J53">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated schedule and renamed info handler
</commit_message>
<xml_diff>
--- a/asuschedule/document.xlsx
+++ b/asuschedule/document.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\ASU_Schedule\asuschedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75C742F-3DED-4B78-BE81-0F0A7A0671D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221A1AF4-C183-4C6C-82E4-438CCC8A4892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-504" yWindow="1332" windowWidth="17280" windowHeight="8880" tabRatio="500" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2489" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2490" uniqueCount="200">
   <si>
     <t>Курс</t>
   </si>
@@ -2447,7 +2447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C2F2DF-FE59-47D0-BDF3-50F27700A4C2}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B25" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -3673,7 +3673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC10DB3-35FC-4C6A-8252-97FB7BCAAC35}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -4728,7 +4728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059CF91E-6117-45C5-82C8-C939713C8D5E}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -11007,7 +11007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
@@ -12348,8 +12348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="D23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12994,8 +12994,8 @@
       <c r="G23" t="s">
         <v>86</v>
       </c>
-      <c r="H23">
-        <v>327</v>
+      <c r="H23" t="s">
+        <v>31</v>
       </c>
       <c r="I23" t="s">
         <v>14</v>
@@ -13840,7 +13840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A50098D-1ABF-4068-8B74-18169C8AD7A1}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>

</xml_diff>